<commit_message>
smal change in completion text
</commit_message>
<xml_diff>
--- a/public/Spreadsheets/municipalityOverview.xlsx
+++ b/public/Spreadsheets/municipalityOverview.xlsx
@@ -23,10 +23,10 @@
     <t>Total revenue</t>
   </si>
   <si>
-    <t>Total yield</t>
-  </si>
-  <si>
-    <t>Total surplus</t>
+    <t>Total yield (KWH)</t>
+  </si>
+  <si>
+    <t>Total surplus (KWH)</t>
   </si>
   <si>
     <t>Zaanstad</t>
@@ -422,8 +422,8 @@
   <cols>
     <col min="1" max="1" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="23.423" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>